<commit_message>
Implements subranges for capacity additions
</commit_message>
<xml_diff>
--- a/InputData/elec/ESUfR/Elec Sources Used for Reliability.xlsx
+++ b/InputData/elec/ESUfR/Elec Sources Used for Reliability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\ESUfR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E863F7EF-789A-4B50-BD5A-B068BF189DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80073164-E0F7-4E79-BD94-769769B28863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24705" yWindow="5655" windowWidth="21840" windowHeight="15600" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>ESUFR Electricity Sources Used for Reliability</t>
   </si>
@@ -60,9 +60,6 @@
     <t>hydrogen combined cycle es</t>
   </si>
   <si>
-    <t>-&gt; electricity source within all fuels</t>
-  </si>
-  <si>
     <t>hard coal es</t>
   </si>
   <si>
@@ -130,6 +127,33 @@
   </si>
   <si>
     <t>hydrogen combustion turbine es</t>
+  </si>
+  <si>
+    <t>Electricity Sources (no es)</t>
+  </si>
+  <si>
+    <t>natural gas combined cycle</t>
+  </si>
+  <si>
+    <t>onshore wind</t>
+  </si>
+  <si>
+    <t>solar PV</t>
+  </si>
+  <si>
+    <t>petroleum</t>
+  </si>
+  <si>
+    <t>natural gas peaker</t>
+  </si>
+  <si>
+    <t>small modular reactor</t>
+  </si>
+  <si>
+    <t>hydrogen combustion turbine</t>
+  </si>
+  <si>
+    <t>hydrogen combined cycle</t>
   </si>
 </sst>
 </file>
@@ -490,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1D3264-BEAA-43D0-A5CC-06C5D3B72BE0}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A34"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,127 +550,122 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -659,10 +678,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="C29:D29"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,49 +689,156 @@
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="B2" t="str">
+        <f>IF(A2="","",CONCATENATE(A2," es"))</f>
+        <v>natural gas combined cycle es</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B21" si="0">IF(A3="","",CONCATENATE(A3," es"))</f>
+        <v>onshore wind es</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>solar PV es</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>petroleum es</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>natural gas peaker es</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>small modular reactor es</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>hydrogen combustion turbine es</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>39</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>hydrogen combined cycle es</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>